<commit_message>
Add class and constructor comments
</commit_message>
<xml_diff>
--- a/test/recording/recording/results/TestWorkbook.xlsx
+++ b/test/recording/recording/results/TestWorkbook.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="10380" windowWidth="19380" xWindow="-90" yWindow="-90"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
@@ -18,8 +18,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt formatCode="yyyy\-mm\-dd\ h:mm:ss" numFmtId="164"/>
-    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="165"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -191,38 +191,38 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="24">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="3" fontId="2" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="4" fontId="2" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="2" fillId="5" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="2" fillId="5" fontId="3" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="2" fillId="6" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="2" fillId="6" fontId="3" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="3" fillId="7" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="3" fillId="7" fontId="4" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="3" fillId="8" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="3" fillId="8" fontId="4" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="4" fillId="9" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="4" fillId="9" fontId="5" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="4" fillId="9" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="4" fillId="10" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="4" fillId="10" fontId="5" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="5" fillId="11" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="5" fillId="11" fontId="6" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="5" fillId="11" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="5" fillId="12" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="5" fillId="12" fontId="6" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="5" fillId="9" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="5" fillId="10" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="6" fillId="11" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="6" fillId="12" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -553,12 +553,12 @@
           </marker>
           <xVal>
             <numRef>
-              <f>'TestSheet2'!$F$3:$F$19</f>
+              <f>'TestSheet2'!$F$3:$F$20</f>
             </numRef>
           </xVal>
           <yVal>
             <numRef>
-              <f>'TestSheet2'!$B$3:$B$19</f>
+              <f>'TestSheet2'!$B$3:$B$20</f>
             </numRef>
           </yVal>
         </ser>
@@ -663,12 +663,12 @@
           </marker>
           <xVal>
             <numRef>
-              <f>'TestSheet2'!$G$3:$G$19</f>
+              <f>'TestSheet2'!$G$3:$G$20</f>
             </numRef>
           </xVal>
           <yVal>
             <numRef>
-              <f>'TestSheet2'!$B$3:$B$19</f>
+              <f>'TestSheet2'!$B$3:$B$20</f>
             </numRef>
           </yVal>
         </ser>
@@ -1124,7 +1124,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.75"/>
   <sheetData/>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1134,7 +1134,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:I19"/>
+  <dimension ref="A2:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1142,15 +1142,15 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.75"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="4"/>
-    <col customWidth="1" max="2" min="2" width="13"/>
-    <col customWidth="1" max="3" min="3" width="17"/>
-    <col customWidth="1" max="4" min="4" width="21"/>
-    <col customWidth="1" max="6" min="5" width="13"/>
-    <col customWidth="1" max="6" min="6" width="13"/>
-    <col customWidth="1" max="7" min="7" width="15"/>
-    <col customWidth="1" max="8" min="8" width="13"/>
-    <col customWidth="1" max="9" min="9" width="26"/>
+    <col width="4" customWidth="1" min="1" max="1"/>
+    <col width="13" customWidth="1" min="2" max="2"/>
+    <col width="17" customWidth="1" min="3" max="3"/>
+    <col width="21" customWidth="1" min="4" max="4"/>
+    <col width="13" customWidth="1" min="5" max="6"/>
+    <col width="13" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
+    <col width="13" customWidth="1" min="8" max="8"/>
+    <col width="26" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -1671,8 +1671,36 @@
         <v>44629.55517581019</v>
       </c>
     </row>
+    <row r="20">
+      <c r="B20" s="22" t="n">
+        <v>1021</v>
+      </c>
+      <c r="C20" s="22" t="n">
+        <v>37.99213457107544</v>
+      </c>
+      <c r="D20" s="22" t="n">
+        <v>250</v>
+      </c>
+      <c r="E20" s="22" t="inlineStr">
+        <is>
+          <t>[1300, 700]</t>
+        </is>
+      </c>
+      <c r="F20" s="22" t="n">
+        <v>79</v>
+      </c>
+      <c r="G20" s="22" t="n">
+        <v>9</v>
+      </c>
+      <c r="H20" s="22" t="n">
+        <v>100</v>
+      </c>
+      <c r="I20" s="23" t="n">
+        <v>44730.3049113426</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -1683,7 +1711,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:H3"/>
+  <dimension ref="B2:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1691,12 +1719,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.75"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="4"/>
-    <col customWidth="1" max="4" min="2" width="13"/>
-    <col customWidth="1" max="5" min="5" width="21"/>
-    <col customWidth="1" max="6" min="6" width="13"/>
-    <col customWidth="1" max="7" min="7" width="15"/>
-    <col customWidth="1" max="8" min="8" width="13"/>
+    <col width="4" customWidth="1" min="1" max="1"/>
+    <col width="13" customWidth="1" min="2" max="4"/>
+    <col width="21" customWidth="1" min="5" max="5"/>
+    <col width="13" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
+    <col width="13" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -1743,31 +1771,55 @@
         </is>
       </c>
       <c r="C3" s="21">
-        <f>AVERAGE('TestSheet2'!B3:B19)</f>
+        <f>AVERAGE('TestSheet2'!B3:B20)</f>
         <v/>
       </c>
       <c r="D3" s="21">
-        <f>AVERAGE('TestSheet2'!C3:C19)</f>
+        <f>AVERAGE('TestSheet2'!C3:C20)</f>
         <v/>
       </c>
       <c r="E3" s="21">
-        <f>AVERAGE('TestSheet2'!D3:D19)</f>
+        <f>AVERAGE('TestSheet2'!D3:D20)</f>
         <v/>
       </c>
       <c r="F3" s="21">
-        <f>AVERAGE('TestSheet2'!F3:F19)</f>
+        <f>AVERAGE('TestSheet2'!F3:F20)</f>
         <v/>
       </c>
       <c r="G3" s="21">
-        <f>AVERAGE('TestSheet2'!G3:G19)</f>
+        <f>AVERAGE('TestSheet2'!G3:G20)</f>
         <v/>
       </c>
       <c r="H3" s="21">
-        <f>AVERAGE('TestSheet2'!H3:H19)</f>
+        <f>AVERAGE('TestSheet2'!H3:H20)</f>
         <v/>
       </c>
+      <c r="I3" s="21">
+        <f>IFERROR(STDEV(TestSheet2!B3:B20)/4.242640687119285,0)</f>
+        <v/>
+      </c>
+      <c r="J3" s="21">
+        <f>IFERROR(STDEV(TestSheet2!C3:C20)/4.242640687119285,0)</f>
+        <v/>
+      </c>
+      <c r="K3" s="21">
+        <f>IFERROR(STDEV(TestSheet2!D3:D20)/4.242640687119285,0)</f>
+        <v/>
+      </c>
+      <c r="L3" s="21">
+        <f>IFERROR(STDEV(TestSheet2!F3:F20)/4.242640687119285,0)</f>
+        <v/>
+      </c>
+      <c r="M3" s="21">
+        <f>IFERROR(STDEV(TestSheet2!G3:G20)/4.242640687119285,0)</f>
+        <v/>
+      </c>
+      <c r="N3" s="21">
+        <f>IFERROR(STDEV(TestSheet2!H3:H20)/4.242640687119285,0)</f>
+        <v/>
+      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>